<commit_message>
Updated BOM for Camera System
</commit_message>
<xml_diff>
--- a/Interfacing/BOM.xlsx
+++ b/Interfacing/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9510 i9\Desktop\Network_Enabled_Camera_Trap\Interfacing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Desktop\Network_Enabled_Camera_Trap\Interfacing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B38A167-24A0-4D35-AF65-9BABEEE6A34F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5864B45D-B095-45E5-B6F1-3C4A00019F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="36" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>ESP32-CAM: WIFI + BLUETOOTH CAMERA DEVELOPMENT BOARD</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Passive Infra-Red (PIR) Sensor HC-SR501</t>
+  </si>
+  <si>
+    <t>Temperature and Humidity Sensor DHT11</t>
   </si>
 </sst>
 </file>
@@ -75,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +104,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,12 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -135,6 +147,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,45 +448,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -491,6 +507,46 @@
       <c r="F5" s="1">
         <f>D5*E5</f>
         <v>229.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>33.909999999999997</v>
+      </c>
+      <c r="F7" s="1">
+        <v>33.909999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated image transmission and processing
</commit_message>
<xml_diff>
--- a/Interfacing/BOM.xlsx
+++ b/Interfacing/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Desktop\Network_Enabled_Camera_Trap\Interfacing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9510 i9\Desktop\Desktop\Network_Enabled_Camera_Trap\Interfacing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5864B45D-B095-45E5-B6F1-3C4A00019F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474B5607-F560-4C5E-99B6-8C7349AB89B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,10 +147,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,24 +448,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -516,7 +516,7 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D6">
@@ -547,6 +547,12 @@
       </c>
       <c r="F7" s="1">
         <v>33.909999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="1">
+        <f>SUM(F5:F7)</f>
+        <v>289.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>